<commit_message>
10/09/2020: Created Registration Test Case
</commit_message>
<xml_diff>
--- a/YourLogoRegressionAutomationTest/src/test/java/selenium/framework/testdata/TestData3.xlsx
+++ b/YourLogoRegressionAutomationTest/src/test/java/selenium/framework/testdata/TestData3.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation tools\Selenium\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="2175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Title</t>
   </si>
@@ -81,6 +77,12 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>rojantest3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -399,26 +401,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,31 +432,34 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -464,27 +470,30 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>36861</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>12345</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>9876543210</v>
       </c>
     </row>

</xml_diff>